<commit_message>
finalizing example for class
</commit_message>
<xml_diff>
--- a/documentation/data_dictionary.xlsx
+++ b/documentation/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/smarte4_illinois_edu/Documents/HK_513/hk513_fall24_repro_deliverable/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B423305-C3B5-D94F-A09A-BD61295BDB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{9B423305-C3B5-D94F-A09A-BD61295BDB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98B212F6-4D88-9F43-B397-D2B4A8D4226F}"/>
   <bookViews>
     <workbookView xWindow="-33180" yWindow="1060" windowWidth="28040" windowHeight="16940" xr2:uid="{D2D333A9-448F-B54C-9654-3812AE5F21F8}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
         <v>50</v>
@@ -667,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -687,7 +687,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
         <v>50</v>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="s">
         <v>50</v>
@@ -727,7 +727,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="s">
         <v>50</v>
@@ -747,7 +747,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
         <v>50</v>
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="s">
         <v>50</v>

</xml_diff>